<commit_message>
Bug fixed realted to Import excel in faeture Master
</commit_message>
<xml_diff>
--- a/configuratior/src/assets/data/json/FeatureMaster.xlsx
+++ b/configuratior/src/assets/data/json/FeatureMaster.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>FeatureCode</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>PicturePath</t>
-  </si>
-  <si>
-    <t>CreatedUser</t>
   </si>
   <si>
     <t>Accessory</t>
@@ -377,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +391,7 @@
     <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,9 +421,6 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel changes for feature/model
</commit_message>
<xml_diff>
--- a/configuratior/src/assets/data/json/FeatureMaster.xlsx
+++ b/configuratior/src/assets/data/json/FeatureMaster.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>FeatureCode</t>
   </si>
   <si>
-    <t>DisplayName</t>
-  </si>
-  <si>
     <t>FeatureDesc</t>
   </si>
   <si>
@@ -36,36 +33,26 @@
     <t>Type</t>
   </si>
   <si>
-    <t>FeatureStatus</t>
-  </si>
-  <si>
-    <t>ModelTemplateItem</t>
-  </si>
-  <si>
-    <t>ItemCodeGenerationRef</t>
-  </si>
-  <si>
     <t>PicturePath</t>
   </si>
   <si>
     <t>Accessory</t>
+  </si>
+  <si>
+    <t>FeatureName</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,9 +78,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,36 +377,30 @@
     <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>